<commit_message>
Feat: Default page completed
</commit_message>
<xml_diff>
--- a/lab03_minesweeper/TouchGFX/assets/texts/texts.xlsx
+++ b/lab03_minesweeper/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2052" uniqueCount="90">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -261,6 +261,30 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;c&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;text&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-9,a-z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0123456789</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right</t>
   </si>
 </sst>
 </file>
@@ -1506,7 +1530,9 @@
       <c r="H4" t="s">
         <v>79</v>
       </c>
-      <c r="I4"/>
+      <c r="I4" t="s">
+        <v>85</v>
+      </c>
       <c r="J4"/>
       <c r="L4" s="4" t="s">
         <v>9</v>
@@ -1969,7 +1995,7 @@
         <v>38</v>
       </c>
       <c r="D18" t="s">
-        <v>66</v>
+        <v>89</v>
       </c>
       <c r="E18" t="s">
         <v>44</v>
@@ -1980,7 +2006,7 @@
     </row>
     <row r="19">
       <c r="B19" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="C19" t="s">
         <v>38</v>
@@ -1992,12 +2018,12 @@
         <v>44</v>
       </c>
       <c r="F19" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C20" t="s">
         <v>38</v>
@@ -2009,43 +2035,44 @@
         <v>44</v>
       </c>
       <c r="F20" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C21" t="s">
         <v>38</v>
       </c>
       <c r="D21" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="E21" t="s">
         <v>44</v>
       </c>
       <c r="F21" t="s">
-        <v>46</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22">
       <c r="B22" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C22" t="s">
         <v>38</v>
       </c>
       <c r="D22" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="E22" t="s">
         <v>44</v>
       </c>
       <c r="F22" t="s">
-        <v>81</v>
-      </c>
-    </row>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Feat: First grid button event completed
</commit_message>
<xml_diff>
--- a/lab03_minesweeper/TouchGFX/assets/texts/texts.xlsx
+++ b/lab03_minesweeper/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2052" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2182" uniqueCount="90">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -2012,7 +2012,7 @@
         <v>38</v>
       </c>
       <c r="D19" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="E19" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
Feat: All function completed
</commit_message>
<xml_diff>
--- a/lab03_minesweeper/TouchGFX/assets/texts/texts.xlsx
+++ b/lab03_minesweeper/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2182" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2590" uniqueCount="92">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -285,6 +285,12 @@
   </si>
   <si>
     <t xml:space="preserve">Right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-9,a-z,A-Z</t>
   </si>
 </sst>
 </file>
@@ -1531,7 +1537,7 @@
         <v>79</v>
       </c>
       <c r="I4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="J4"/>
       <c r="L4" s="4" t="s">
@@ -2072,7 +2078,23 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23"/>
+    <row r="23">
+      <c r="B23" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" t="s">
+        <v>44</v>
+      </c>
+      <c r="F23" t="s">
+        <v>83</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>